<commit_message>
add lec 12 slides/videos
</commit_message>
<xml_diff>
--- a/courses/cnns-xmuf21/files/grading/19级网安课程名单.xlsx
+++ b/courses/cnns-xmuf21/files/grading/19级网安课程名单.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\iCloudDrive\博士期间\博士课程\计算机网络与安全\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5752EF-90CF-4023-8817-1B55ACA666B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB4AC6-1C65-44B4-9B13-CE9BF08609FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7812" yWindow="456" windowWidth="4356" windowHeight="3096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8928" yWindow="456" windowWidth="4356" windowHeight="3096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="汇总" sheetId="1" r:id="rId1"/>
@@ -301,15 +301,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>最低分：43.5</t>
+    <t>平均分：84.39</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>最高分：88.5</t>
+    <t>最低分：57</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>平均分：75.14</t>
+    <t>最高分：94</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -391,22 +391,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>542185</xdr:colOff>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>119455</xdr:rowOff>
+      <xdr:rowOff>117818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>535879</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>136976</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="图片 5">
+        <xdr:cNvPr id="3" name="图片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28D6D037-E7EC-4DC5-BAED-B89908314476}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FA12AF-5293-408C-8012-C48DEA7F89E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -429,8 +429,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4916065" y="8166175"/>
-          <a:ext cx="3613194" cy="2760721"/>
+          <a:off x="4396740" y="8164538"/>
+          <a:ext cx="4015740" cy="3067342"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44:P44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -872,7 +872,7 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11">
-        <v>77.5</v>
+        <v>84.5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -926,7 +926,7 @@
       </c>
       <c r="I12" s="1"/>
       <c r="J12">
-        <v>78.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
       </c>
       <c r="I13" s="1"/>
       <c r="J13">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
       </c>
       <c r="I14" s="1"/>
       <c r="J14">
-        <v>86.5</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="I16" s="1"/>
       <c r="J16">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="I17" s="1"/>
       <c r="J17">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="I18" s="1"/>
       <c r="J18">
-        <v>67.5</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="I19" s="1"/>
       <c r="J19">
-        <v>43.5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="I20" s="1"/>
       <c r="J20">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="I21" s="1"/>
       <c r="J21">
-        <v>73.5</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="I22" s="1"/>
       <c r="J22">
-        <v>78.5</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="I23" s="1"/>
       <c r="J23">
-        <v>70.5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="I24" s="1"/>
       <c r="J24">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="I25" s="2"/>
       <c r="J25">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="I26" s="1"/>
       <c r="J26">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="I27" s="1"/>
       <c r="J27">
-        <v>83.5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="I28" s="1"/>
       <c r="J28">
-        <v>88.5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="I29" s="1"/>
       <c r="J29">
-        <v>70.5</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="I30" s="1"/>
       <c r="J30">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="I31" s="1"/>
       <c r="J31">
-        <v>86</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="I33" s="1"/>
       <c r="J33">
-        <v>81.5</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="I34" s="1"/>
       <c r="J34">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="I35" s="1"/>
       <c r="J35">
-        <v>85.5</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="I36" s="1"/>
       <c r="J36">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="I37" s="1"/>
       <c r="J37">
-        <v>78.5</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="I38" s="1"/>
       <c r="J38">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="I39" s="1"/>
       <c r="J39">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="J40">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1707,12 +1707,12 @@
       </c>
       <c r="I41" s="1"/>
       <c r="J41">
-        <v>78.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1723,12 +1723,12 @@
         <v>89</v>
       </c>
       <c r="J43" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>